<commit_message>
Fix file paths and remove unnecessary code
</commit_message>
<xml_diff>
--- a/FicherosEntrada/2024/Exportaciones-MELILLA-01-07/01-07/Oferta-FP-24-25_MELILLA_vacantes_01-07_JSJ.xlsx
+++ b/FicherosEntrada/2024/Exportaciones-MELILLA-01-07/01-07/Oferta-FP-24-25_MELILLA_vacantes_01-07_JSJ.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GB" sheetId="1" state="visible" r:id="rId2"/>
@@ -938,7 +938,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1069,6 +1069,10 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1275,7 +1279,7 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1581,8 +1585,8 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.01171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1969,7 +1973,7 @@
   </sheetPr>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -2929,8 +2933,8 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.01171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3093,15 +3097,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" s="32" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="32" t="n">
         <v>52000403</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="32" t="n">
-        <v>122106061</v>
+      <c r="C10" s="33" t="n">
+        <v>122106064</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>96</v>
@@ -3178,15 +3182,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>52000658</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="4" t="n">
-        <v>122123054</v>
+      <c r="C15" s="33" t="n">
+        <v>122107014</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>101</v>
@@ -3297,15 +3301,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
         <v>52000701</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="4" t="n">
-        <v>122123644</v>
+      <c r="C22" s="33" t="n">
+        <v>122105024</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>107</v>
@@ -3315,8 +3319,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="33"/>
-      <c r="D24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="D24" s="35"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3336,7 +3340,7 @@
   </sheetPr>
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H71" activeCellId="0" sqref="H71"/>
     </sheetView>
   </sheetViews>
@@ -3358,7 +3362,7 @@
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
@@ -3588,10 +3592,10 @@
       <c r="D8" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="36" t="n">
+      <c r="E8" s="37" t="n">
         <v>31708</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="38" t="s">
         <v>116</v>
       </c>
       <c r="G8" s="22" t="n">
@@ -3600,7 +3604,7 @@
       <c r="H8" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I8" s="36" t="n">
+      <c r="I8" s="37" t="n">
         <v>31708</v>
       </c>
       <c r="J8" s="15" t="n">
@@ -3620,7 +3624,7 @@
       <c r="D9" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="38" t="n">
+      <c r="E9" s="39" t="n">
         <v>30179</v>
       </c>
       <c r="F9" s="20" t="s">
@@ -3632,7 +3636,7 @@
       <c r="H9" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I9" s="38" t="n">
+      <c r="I9" s="39" t="n">
         <v>30179</v>
       </c>
       <c r="J9" s="15" t="n">
@@ -3864,630 +3868,630 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="39" t="n">
+      <c r="A17" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="40" t="n">
+      <c r="E17" s="41" t="n">
         <v>31367</v>
       </c>
-      <c r="F17" s="41" t="s">
+      <c r="F17" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="G17" s="39" t="n">
+      <c r="G17" s="40" t="n">
         <v>200</v>
       </c>
       <c r="H17" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I17" s="40" t="s">
+      <c r="I17" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="J17" s="39" t="n">
+      <c r="J17" s="40" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="39" t="n">
+      <c r="A18" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E18" s="40" t="n">
+      <c r="E18" s="41" t="n">
         <v>31368</v>
       </c>
-      <c r="F18" s="41" t="s">
+      <c r="F18" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="G18" s="39" t="n">
+      <c r="G18" s="40" t="n">
         <v>190</v>
       </c>
       <c r="H18" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I18" s="40" t="s">
+      <c r="I18" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="J18" s="39" t="n">
+      <c r="J18" s="40" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="39" t="n">
+      <c r="A19" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E19" s="40" t="n">
+      <c r="E19" s="41" t="n">
         <v>31370</v>
       </c>
-      <c r="F19" s="41" t="s">
+      <c r="F19" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="G19" s="39" t="n">
+      <c r="G19" s="40" t="n">
         <v>200</v>
       </c>
       <c r="H19" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I19" s="40" t="s">
+      <c r="I19" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="J19" s="39" t="n">
+      <c r="J19" s="40" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="39" t="n">
+      <c r="A20" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E20" s="40" t="n">
+      <c r="E20" s="41" t="n">
         <v>31369</v>
       </c>
-      <c r="F20" s="41" t="s">
+      <c r="F20" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="G20" s="39" t="n">
+      <c r="G20" s="40" t="n">
         <v>200</v>
       </c>
       <c r="H20" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I20" s="40" t="s">
+      <c r="I20" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="J20" s="39" t="n">
+      <c r="J20" s="40" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="39" t="n">
+      <c r="A21" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E21" s="40" t="n">
+      <c r="E21" s="41" t="n">
         <v>31709</v>
       </c>
-      <c r="F21" s="41" t="s">
+      <c r="F21" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="42" t="n">
+      <c r="G21" s="43" t="n">
         <v>100</v>
       </c>
       <c r="H21" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I21" s="40" t="n">
+      <c r="I21" s="41" t="n">
         <v>31709</v>
       </c>
-      <c r="J21" s="39" t="n">
+      <c r="J21" s="40" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="39" t="n">
+      <c r="A22" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E22" s="40" t="n">
+      <c r="E22" s="41" t="n">
         <v>31664</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="G22" s="42" t="n">
+      <c r="G22" s="43" t="n">
         <v>35</v>
       </c>
       <c r="H22" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I22" s="40" t="n">
+      <c r="I22" s="41" t="n">
         <v>31664</v>
       </c>
-      <c r="J22" s="39" t="n">
+      <c r="J22" s="40" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="39" t="n">
+      <c r="A23" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E23" s="40" t="n">
+      <c r="E23" s="41" t="n">
         <v>30156</v>
       </c>
-      <c r="F23" s="41" t="s">
+      <c r="F23" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="G23" s="42" t="n">
+      <c r="G23" s="43" t="n">
         <v>70</v>
       </c>
       <c r="H23" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I23" s="40" t="n">
+      <c r="I23" s="41" t="n">
         <v>30156</v>
       </c>
-      <c r="J23" s="39" t="n">
+      <c r="J23" s="40" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="39" t="n">
+      <c r="A24" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E24" s="40" t="n">
+      <c r="E24" s="41" t="n">
         <v>31371</v>
       </c>
-      <c r="F24" s="41" t="s">
+      <c r="F24" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="G24" s="39" t="n">
+      <c r="G24" s="40" t="n">
         <v>170</v>
       </c>
       <c r="H24" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I24" s="40" t="s">
+      <c r="I24" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="J24" s="39" t="n">
+      <c r="J24" s="40" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="39" t="n">
+      <c r="A25" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D25" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E25" s="40" t="n">
+      <c r="E25" s="41" t="n">
         <v>31372</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="G25" s="39" t="n">
+      <c r="G25" s="40" t="n">
         <v>100</v>
       </c>
       <c r="H25" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I25" s="40" t="s">
+      <c r="I25" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="J25" s="39" t="n">
+      <c r="J25" s="40" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B26" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="39" t="n">
+      <c r="A26" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D26" s="39" t="s">
+      <c r="D26" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E26" s="40" t="n">
+      <c r="E26" s="41" t="n">
         <v>31373</v>
       </c>
-      <c r="F26" s="39" t="s">
+      <c r="F26" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="G26" s="39" t="n">
+      <c r="G26" s="40" t="n">
         <v>145</v>
       </c>
       <c r="H26" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I26" s="40" t="s">
+      <c r="I26" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="J26" s="39" t="n">
+      <c r="J26" s="40" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="39" t="n">
+      <c r="A27" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D27" s="39" t="s">
+      <c r="D27" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E27" s="40" t="n">
+      <c r="E27" s="41" t="n">
         <v>31374</v>
       </c>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="G27" s="39" t="n">
+      <c r="G27" s="40" t="n">
         <v>145</v>
       </c>
       <c r="H27" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I27" s="40" t="s">
+      <c r="I27" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="J27" s="39" t="n">
+      <c r="J27" s="40" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="39" t="n">
+      <c r="A28" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D28" s="39" t="s">
+      <c r="D28" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="40" t="n">
+      <c r="E28" s="41" t="n">
         <v>31378</v>
       </c>
-      <c r="F28" s="39" t="s">
+      <c r="F28" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="G28" s="39" t="n">
+      <c r="G28" s="40" t="n">
         <v>400</v>
       </c>
       <c r="H28" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I28" s="40" t="s">
+      <c r="I28" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="J28" s="39" t="n">
+      <c r="J28" s="40" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="39" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="39" t="n">
+      <c r="A29" s="40" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="40" t="n">
         <v>122106083</v>
       </c>
-      <c r="D29" s="39" t="s">
+      <c r="D29" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E29" s="40" t="n">
+      <c r="E29" s="41" t="n">
         <v>31375</v>
       </c>
-      <c r="F29" s="39" t="s">
+      <c r="F29" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="G29" s="39" t="n">
+      <c r="G29" s="40" t="n">
         <v>40</v>
       </c>
       <c r="H29" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I29" s="40" t="s">
+      <c r="I29" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="J29" s="39" t="n">
+      <c r="J29" s="40" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B30" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="43" t="n">
+      <c r="A30" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D30" s="43" t="s">
+      <c r="D30" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E30" s="44" t="s">
+      <c r="E30" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="F30" s="43" t="s">
+      <c r="F30" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="G30" s="45" t="n">
+      <c r="G30" s="46" t="n">
         <v>160</v>
       </c>
       <c r="H30" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I30" s="44" t="s">
+      <c r="I30" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="J30" s="43" t="n">
+      <c r="J30" s="44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B31" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="43" t="n">
+      <c r="A31" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D31" s="43" t="s">
+      <c r="D31" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E31" s="44" t="s">
+      <c r="E31" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="F31" s="43" t="s">
+      <c r="F31" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="G31" s="45" t="n">
+      <c r="G31" s="46" t="n">
         <v>260</v>
       </c>
       <c r="H31" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I31" s="44" t="s">
+      <c r="I31" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="J31" s="43" t="n">
+      <c r="J31" s="44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B32" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="43" t="n">
+      <c r="A32" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D32" s="43" t="s">
+      <c r="D32" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E32" s="44" t="s">
+      <c r="E32" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="F32" s="43" t="s">
+      <c r="F32" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="G32" s="43" t="n">
+      <c r="G32" s="44" t="n">
         <v>200</v>
       </c>
       <c r="H32" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I32" s="44" t="s">
+      <c r="I32" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="J32" s="43" t="n">
+      <c r="J32" s="44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="43" t="n">
+      <c r="A33" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D33" s="43" t="s">
+      <c r="D33" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E33" s="44" t="s">
+      <c r="E33" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="F33" s="43" t="s">
+      <c r="F33" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="G33" s="43" t="n">
+      <c r="G33" s="44" t="n">
         <v>170</v>
       </c>
       <c r="H33" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I33" s="44" t="s">
+      <c r="I33" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="J33" s="43" t="n">
+      <c r="J33" s="44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="43" t="n">
+      <c r="A34" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D34" s="43" t="s">
+      <c r="D34" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E34" s="44" t="n">
+      <c r="E34" s="45" t="n">
         <v>31709</v>
       </c>
-      <c r="F34" s="43" t="s">
+      <c r="F34" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="G34" s="43" t="n">
+      <c r="G34" s="44" t="n">
         <v>100</v>
       </c>
       <c r="H34" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I34" s="44" t="n">
+      <c r="I34" s="45" t="n">
         <v>31709</v>
       </c>
-      <c r="J34" s="43" t="n">
+      <c r="J34" s="44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B35" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="43" t="n">
+      <c r="A35" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D35" s="43" t="s">
+      <c r="D35" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E35" s="36" t="n">
+      <c r="E35" s="37" t="n">
         <v>31708</v>
       </c>
-      <c r="F35" s="37" t="s">
+      <c r="F35" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="46" t="n">
+      <c r="G35" s="47" t="n">
         <v>35</v>
       </c>
       <c r="H35" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I35" s="36" t="n">
+      <c r="I35" s="37" t="n">
         <v>31708</v>
       </c>
-      <c r="J35" s="43" t="n">
+      <c r="J35" s="44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B36" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="43" t="n">
+      <c r="A36" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B36" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D36" s="43" t="s">
+      <c r="D36" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E36" s="38" t="n">
+      <c r="E36" s="39" t="n">
         <v>30179</v>
       </c>
-      <c r="F36" s="37" t="s">
+      <c r="F36" s="38" t="s">
         <v>65</v>
       </c>
       <c r="G36" s="18" t="n">
@@ -4496,266 +4500,266 @@
       <c r="H36" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I36" s="38" t="n">
+      <c r="I36" s="39" t="n">
         <v>30179</v>
       </c>
-      <c r="J36" s="43" t="n">
+      <c r="J36" s="44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B37" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="43" t="n">
+      <c r="A37" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B37" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D37" s="43" t="s">
+      <c r="D37" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E37" s="44" t="s">
+      <c r="E37" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="F37" s="43" t="s">
+      <c r="F37" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="G37" s="43" t="n">
+      <c r="G37" s="44" t="n">
         <v>160</v>
       </c>
       <c r="H37" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I37" s="44" t="s">
+      <c r="I37" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="J37" s="43" t="n">
+      <c r="J37" s="44" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B38" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="43" t="n">
+      <c r="A38" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B38" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E38" s="44" t="s">
+      <c r="E38" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="F38" s="43" t="s">
+      <c r="F38" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="G38" s="43" t="n">
+      <c r="G38" s="44" t="n">
         <v>100</v>
       </c>
       <c r="H38" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I38" s="44" t="s">
+      <c r="I38" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="J38" s="43" t="n">
+      <c r="J38" s="44" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B39" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="43" t="n">
+      <c r="A39" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B39" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D39" s="43" t="s">
+      <c r="D39" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E39" s="44" t="s">
+      <c r="E39" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="F39" s="43" t="s">
+      <c r="F39" s="44" t="s">
         <v>166</v>
       </c>
-      <c r="G39" s="43" t="n">
+      <c r="G39" s="44" t="n">
         <v>100</v>
       </c>
       <c r="H39" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I39" s="44" t="s">
+      <c r="I39" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="J39" s="43" t="n">
+      <c r="J39" s="44" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B40" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="43" t="n">
+      <c r="A40" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B40" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D40" s="43" t="s">
+      <c r="D40" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E40" s="44" t="s">
+      <c r="E40" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="F40" s="43" t="s">
+      <c r="F40" s="44" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="43" t="n">
+      <c r="G40" s="44" t="n">
         <v>100</v>
       </c>
       <c r="H40" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I40" s="44" t="s">
+      <c r="I40" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="J40" s="43" t="n">
+      <c r="J40" s="44" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B41" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="43" t="n">
+      <c r="A41" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B41" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D41" s="43" t="s">
+      <c r="D41" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E41" s="44" t="s">
+      <c r="E41" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="F41" s="43" t="s">
+      <c r="F41" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="G41" s="43" t="n">
+      <c r="G41" s="44" t="n">
         <v>60</v>
       </c>
       <c r="H41" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I41" s="44" t="s">
+      <c r="I41" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="J41" s="43" t="n">
+      <c r="J41" s="44" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B42" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" s="43" t="n">
+      <c r="A42" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B42" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D42" s="43" t="s">
+      <c r="D42" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E42" s="44" t="s">
+      <c r="E42" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="F42" s="43" t="s">
+      <c r="F42" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="G42" s="43" t="n">
+      <c r="G42" s="44" t="n">
         <v>400</v>
       </c>
       <c r="H42" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I42" s="44" t="s">
+      <c r="I42" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="J42" s="43" t="n">
+      <c r="J42" s="44" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="43" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B43" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="43" t="n">
+      <c r="A43" s="44" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B43" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="44" t="n">
         <v>122123013</v>
       </c>
-      <c r="D43" s="43" t="s">
+      <c r="D43" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E43" s="44" t="s">
+      <c r="E43" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="F43" s="43" t="s">
+      <c r="F43" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="G43" s="43" t="n">
+      <c r="G43" s="44" t="n">
         <v>40</v>
       </c>
       <c r="H43" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I43" s="44" t="s">
+      <c r="I43" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="J43" s="43" t="n">
+      <c r="J43" s="44" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="47" t="n">
-        <v>52000403</v>
-      </c>
-      <c r="B44" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="47" t="n">
+      <c r="A44" s="48" t="n">
+        <v>52000403</v>
+      </c>
+      <c r="B44" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="48" t="n">
         <v>122123013</v>
       </c>
-      <c r="D44" s="47" t="s">
+      <c r="D44" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="E44" s="48" t="s">
+      <c r="E44" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="F44" s="47" t="s">
+      <c r="F44" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="G44" s="47" t="n">
+      <c r="G44" s="48" t="n">
         <v>40</v>
       </c>
       <c r="H44" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I44" s="48" t="s">
+      <c r="I44" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="J44" s="47" t="n">
+      <c r="J44" s="48" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4766,7 +4770,7 @@
       <c r="B45" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C45" s="49" t="n">
+      <c r="C45" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D45" s="28" t="s">
@@ -4798,7 +4802,7 @@
       <c r="B46" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C46" s="49" t="n">
+      <c r="C46" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D46" s="28" t="s">
@@ -4830,7 +4834,7 @@
       <c r="B47" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C47" s="49" t="n">
+      <c r="C47" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D47" s="28" t="s">
@@ -4862,7 +4866,7 @@
       <c r="B48" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C48" s="49" t="n">
+      <c r="C48" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D48" s="28" t="s">
@@ -4894,7 +4898,7 @@
       <c r="B49" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C49" s="49" t="n">
+      <c r="C49" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D49" s="28" t="s">
@@ -4926,7 +4930,7 @@
       <c r="B50" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C50" s="49" t="n">
+      <c r="C50" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D50" s="28" t="s">
@@ -4958,25 +4962,25 @@
       <c r="B51" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C51" s="49" t="n">
+      <c r="C51" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D51" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="E51" s="36" t="n">
+      <c r="E51" s="37" t="n">
         <v>31708</v>
       </c>
-      <c r="F51" s="37" t="s">
+      <c r="F51" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="46" t="n">
+      <c r="G51" s="47" t="n">
         <v>35</v>
       </c>
       <c r="H51" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I51" s="36" t="n">
+      <c r="I51" s="37" t="n">
         <v>31708</v>
       </c>
       <c r="J51" s="28" t="n">
@@ -4990,16 +4994,16 @@
       <c r="B52" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C52" s="49" t="n">
+      <c r="C52" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D52" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="E52" s="38" t="n">
+      <c r="E52" s="39" t="n">
         <v>30179</v>
       </c>
-      <c r="F52" s="37" t="s">
+      <c r="F52" s="38" t="s">
         <v>65</v>
       </c>
       <c r="G52" s="18" t="n">
@@ -5008,7 +5012,7 @@
       <c r="H52" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I52" s="38" t="n">
+      <c r="I52" s="39" t="n">
         <v>30179</v>
       </c>
       <c r="J52" s="28" t="n">
@@ -5022,16 +5026,16 @@
       <c r="B53" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C53" s="49" t="n">
+      <c r="C53" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D53" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="E53" s="50" t="n">
+      <c r="E53" s="51" t="n">
         <v>30339</v>
       </c>
-      <c r="F53" s="51" t="s">
+      <c r="F53" s="52" t="s">
         <v>182</v>
       </c>
       <c r="G53" s="28" t="n">
@@ -5040,7 +5044,7 @@
       <c r="H53" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I53" s="50" t="n">
+      <c r="I53" s="51" t="n">
         <v>30339</v>
       </c>
       <c r="J53" s="28" t="n">
@@ -5054,7 +5058,7 @@
       <c r="B54" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C54" s="49" t="n">
+      <c r="C54" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D54" s="28" t="s">
@@ -5086,7 +5090,7 @@
       <c r="B55" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C55" s="49" t="n">
+      <c r="C55" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D55" s="28" t="s">
@@ -5118,7 +5122,7 @@
       <c r="B56" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C56" s="49" t="n">
+      <c r="C56" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D56" s="28" t="s">
@@ -5150,7 +5154,7 @@
       <c r="B57" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C57" s="49" t="n">
+      <c r="C57" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D57" s="28" t="s">
@@ -5159,7 +5163,7 @@
       <c r="E57" s="29" t="n">
         <v>30017</v>
       </c>
-      <c r="F57" s="51" t="s">
+      <c r="F57" s="52" t="s">
         <v>166</v>
       </c>
       <c r="G57" s="28" t="n">
@@ -5182,28 +5186,28 @@
       <c r="B58" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C58" s="49" t="n">
+      <c r="C58" s="50" t="n">
         <v>122123033</v>
       </c>
       <c r="D58" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="E58" s="52" t="n">
+      <c r="E58" s="53" t="n">
         <v>30347</v>
       </c>
-      <c r="F58" s="53" t="s">
+      <c r="F58" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="G58" s="53" t="n">
+      <c r="G58" s="54" t="n">
         <v>90</v>
       </c>
       <c r="H58" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I58" s="52" t="n">
+      <c r="I58" s="53" t="n">
         <v>30347</v>
       </c>
-      <c r="J58" s="53" t="n">
+      <c r="J58" s="54" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5211,31 +5215,31 @@
       <c r="A59" s="28" t="n">
         <v>52000661</v>
       </c>
-      <c r="B59" s="53" t="s">
+      <c r="B59" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="C59" s="54" t="n">
+      <c r="C59" s="55" t="n">
         <v>122123033</v>
       </c>
-      <c r="D59" s="55" t="s">
+      <c r="D59" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="E59" s="52" t="n">
+      <c r="E59" s="53" t="n">
         <v>30348</v>
       </c>
-      <c r="F59" s="56" t="s">
+      <c r="F59" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="G59" s="53" t="n">
+      <c r="G59" s="54" t="n">
         <v>400</v>
       </c>
       <c r="H59" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I59" s="52" t="n">
+      <c r="I59" s="53" t="n">
         <v>30348</v>
       </c>
-      <c r="J59" s="53" t="n">
+      <c r="J59" s="54" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5255,7 +5259,7 @@
       <c r="E60" s="29" t="n">
         <v>30345</v>
       </c>
-      <c r="F60" s="57" t="s">
+      <c r="F60" s="58" t="s">
         <v>186</v>
       </c>
       <c r="G60" s="28" t="n">
@@ -5275,31 +5279,31 @@
       <c r="A61" s="28" t="n">
         <v>52000661</v>
       </c>
-      <c r="B61" s="58" t="s">
+      <c r="B61" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="C61" s="58" t="n">
+      <c r="C61" s="59" t="n">
         <v>122123043</v>
       </c>
-      <c r="D61" s="58" t="s">
+      <c r="D61" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="E61" s="59" t="n">
+      <c r="E61" s="60" t="n">
         <v>30017</v>
       </c>
-      <c r="F61" s="58" t="s">
+      <c r="F61" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="G61" s="60" t="n">
+      <c r="G61" s="61" t="n">
         <v>100</v>
       </c>
       <c r="H61" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I61" s="59" t="n">
+      <c r="I61" s="60" t="n">
         <v>30017</v>
       </c>
-      <c r="J61" s="58" t="n">
+      <c r="J61" s="59" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5476,19 +5480,19 @@
       <c r="D67" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="E67" s="36" t="n">
+      <c r="E67" s="37" t="n">
         <v>31708</v>
       </c>
-      <c r="F67" s="37" t="s">
+      <c r="F67" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="G67" s="46" t="n">
+      <c r="G67" s="47" t="n">
         <v>35</v>
       </c>
       <c r="H67" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I67" s="36" t="n">
+      <c r="I67" s="37" t="n">
         <v>31708</v>
       </c>
       <c r="J67" s="23" t="n">
@@ -5499,31 +5503,31 @@
       <c r="A68" s="28" t="n">
         <v>52000661</v>
       </c>
-      <c r="B68" s="58" t="s">
+      <c r="B68" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="C68" s="58" t="n">
+      <c r="C68" s="59" t="n">
         <v>122123043</v>
       </c>
-      <c r="D68" s="58" t="s">
+      <c r="D68" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="E68" s="59" t="n">
+      <c r="E68" s="60" t="n">
         <v>30020</v>
       </c>
-      <c r="F68" s="58" t="s">
+      <c r="F68" s="59" t="s">
         <v>174</v>
       </c>
-      <c r="G68" s="58" t="n">
+      <c r="G68" s="59" t="n">
         <v>70</v>
       </c>
       <c r="H68" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="I68" s="59" t="n">
+      <c r="I68" s="60" t="n">
         <v>30020</v>
       </c>
-      <c r="J68" s="58" t="n">
+      <c r="J68" s="59" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5531,31 +5535,31 @@
       <c r="A69" s="28" t="n">
         <v>52000662</v>
       </c>
-      <c r="B69" s="58" t="s">
+      <c r="B69" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="C69" s="58" t="n">
+      <c r="C69" s="59" t="n">
         <v>122123044</v>
       </c>
-      <c r="D69" s="58" t="s">
+      <c r="D69" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="E69" s="59" t="n">
+      <c r="E69" s="60" t="n">
         <v>31709</v>
       </c>
-      <c r="F69" s="58" t="s">
+      <c r="F69" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="G69" s="58" t="n">
+      <c r="G69" s="59" t="n">
         <v>100</v>
       </c>
       <c r="H69" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I69" s="59" t="n">
+      <c r="I69" s="60" t="n">
         <v>31709</v>
       </c>
-      <c r="J69" s="58" t="n">
+      <c r="J69" s="59" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5572,10 +5576,10 @@
       <c r="D70" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="E70" s="38" t="n">
+      <c r="E70" s="39" t="n">
         <v>30179</v>
       </c>
-      <c r="F70" s="37" t="s">
+      <c r="F70" s="38" t="s">
         <v>65</v>
       </c>
       <c r="G70" s="18" t="n">
@@ -5584,7 +5588,7 @@
       <c r="H70" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="I70" s="38" t="n">
+      <c r="I70" s="39" t="n">
         <v>30179</v>
       </c>
       <c r="J70" s="23" t="n">
@@ -5652,7 +5656,7 @@
       <c r="I72" s="24" t="n">
         <v>31401</v>
       </c>
-      <c r="J72" s="58" t="n">
+      <c r="J72" s="59" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5684,7 +5688,7 @@
       <c r="I73" s="24" t="n">
         <v>31403</v>
       </c>
-      <c r="J73" s="58" t="n">
+      <c r="J73" s="59" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5716,7 +5720,7 @@
       <c r="I74" s="24" t="n">
         <v>31406</v>
       </c>
-      <c r="J74" s="58" t="n">
+      <c r="J74" s="59" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5748,7 +5752,7 @@
       <c r="I75" s="26" t="n">
         <v>31410</v>
       </c>
-      <c r="J75" s="58" t="n">
+      <c r="J75" s="59" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5780,7 +5784,7 @@
       <c r="I76" s="24" t="n">
         <v>31407</v>
       </c>
-      <c r="J76" s="58" t="n">
+      <c r="J76" s="59" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5802,7 +5806,7 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -5839,10 +5843,10 @@
       <c r="B2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="61" t="n">
+      <c r="C2" s="62" t="n">
         <v>124120014</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="63" t="s">
         <v>197</v>
       </c>
       <c r="E2" s="10" t="n">
@@ -5901,7 +5905,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5927,7 +5931,7 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>